<commit_message>
Fix online lobby player display and sync
</commit_message>
<xml_diff>
--- a/HentaIto.xlsx
+++ b/HentaIto.xlsx
@@ -10,7 +10,7 @@
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="530" documentId="11_AD4D066CA252ABDACC10488EC9D2E75A73EEDF52" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9A710406-35BC-472E-B569-DAC58B627301}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4230" yWindow="2190" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ゲーム概要" sheetId="1" r:id="rId1"/>
@@ -4103,8 +4103,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D206"/>
   <sheetViews>
-    <sheetView topLeftCell="A94" workbookViewId="0">
-      <selection activeCell="M136" sqref="M136"/>
+    <sheetView tabSelected="1" topLeftCell="A26" workbookViewId="0">
+      <selection activeCell="A33" sqref="A33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75"/>
@@ -4935,7 +4935,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{816F8737-1B4B-4B82-8625-0E9BB4498D5F}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="Z15" sqref="Z15"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Update themes with new abnormal topics and adjust title score thresholds
</commit_message>
<xml_diff>
--- a/HentaIto.xlsx
+++ b/HentaIto.xlsx
@@ -4103,8 +4103,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D206"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A26" workbookViewId="0">
-      <selection activeCell="A33" sqref="A33"/>
+    <sheetView tabSelected="1" topLeftCell="A194" workbookViewId="0">
+      <selection activeCell="A143" sqref="A143"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75"/>

</xml_diff>